<commit_message>
added stochastic seir for log-normal and gamma
</commit_message>
<xml_diff>
--- a/results/primer/VanillaSEIR_Scenario0_Primer_200_log-normal.xlsx
+++ b/results/primer/VanillaSEIR_Scenario0_Primer_200_log-normal.xlsx
@@ -535,19 +535,19 @@
     </row>
     <row r="2" spans="1:30">
       <c r="A2">
-        <v>0.3301124447585448</v>
+        <v>0.329955947548125</v>
       </c>
       <c r="B2">
-        <v>0.3838432362798726</v>
+        <v>0.3835379738755286</v>
       </c>
       <c r="C2">
-        <v>0.2822077631451613</v>
+        <v>0.2821739802348961</v>
       </c>
       <c r="D2">
-        <v>0.3553962275332188</v>
+        <v>0.3549827534312814</v>
       </c>
       <c r="E2">
-        <v>0.3039694276749033</v>
+        <v>0.3038799051185036</v>
       </c>
       <c r="F2">
         <v>7</v>
@@ -565,64 +565,64 @@
         <v>7</v>
       </c>
       <c r="K2">
-        <v>2.310787113309814</v>
+        <v>2.309691632836875</v>
       </c>
       <c r="L2">
-        <v>2.686902653959108</v>
+        <v>2.6847658171287</v>
       </c>
       <c r="M2">
-        <v>1.975454342016129</v>
+        <v>1.975217861644273</v>
       </c>
       <c r="N2">
-        <v>2.487773592732531</v>
+        <v>2.48487927401897</v>
       </c>
       <c r="O2">
-        <v>2.127785993724323</v>
+        <v>2.127159335829525</v>
       </c>
       <c r="P2">
-        <v>175.8811</v>
+        <v>176.00503</v>
       </c>
       <c r="Q2">
-        <v>235.2255678961783</v>
+        <v>234.6407409430736</v>
       </c>
       <c r="R2">
-        <v>134.3538863839666</v>
+        <v>134.4303197968127</v>
       </c>
       <c r="S2">
-        <v>198.8202432661419</v>
+        <v>198.927849887097</v>
       </c>
       <c r="T2">
-        <v>152.1632627017614</v>
+        <v>152.3979670103585</v>
       </c>
       <c r="U2">
-        <v>0.04051437110079735</v>
+        <v>0.04045397268321832</v>
       </c>
       <c r="V2">
-        <v>0.06084649028468512</v>
+        <v>0.06075139190588973</v>
       </c>
       <c r="W2">
-        <v>0.0218242570697878</v>
+        <v>0.021830316360436</v>
       </c>
       <c r="X2">
-        <v>0.05085157498044345</v>
+        <v>0.05074990909545279</v>
       </c>
       <c r="Y2">
-        <v>0.03002462465667989</v>
+        <v>0.03001347679060722</v>
       </c>
       <c r="Z2">
-        <v>0.6765292199944638</v>
+        <v>0.6761959217999651</v>
       </c>
       <c r="AA2">
-        <v>0.7871525444185306</v>
+        <v>0.7867371493239307</v>
       </c>
       <c r="AB2">
-        <v>0.5428245994759742</v>
+        <v>0.5428695047209194</v>
       </c>
       <c r="AC2">
-        <v>0.7366712580662225</v>
+        <v>0.7361708161371121</v>
       </c>
       <c r="AD2">
-        <v>0.6078207728949099</v>
+        <v>0.6077257788357813</v>
       </c>
     </row>
     <row r="3" spans="1:30">
@@ -642,79 +642,79 @@
         <v>0.33</v>
       </c>
       <c r="F3">
-        <v>7.00045286559842</v>
+        <v>6.995053518910998</v>
       </c>
       <c r="G3">
-        <v>8.849310981096261</v>
+        <v>8.839945533553912</v>
       </c>
       <c r="H3">
-        <v>5.460954861440684</v>
+        <v>5.458409058833954</v>
       </c>
       <c r="I3">
-        <v>7.832539620935559</v>
+        <v>7.827740952391174</v>
       </c>
       <c r="J3">
-        <v>6.12978130780996</v>
+        <v>6.128389689880177</v>
       </c>
       <c r="K3">
-        <v>2.310149445647478</v>
+        <v>2.308367661240629</v>
       </c>
       <c r="L3">
-        <v>2.920272623761766</v>
+        <v>2.917182026072791</v>
       </c>
       <c r="M3">
-        <v>1.802115104275426</v>
+        <v>1.801274989415205</v>
       </c>
       <c r="N3">
-        <v>2.584738074908734</v>
+        <v>2.583154514289088</v>
       </c>
       <c r="O3">
-        <v>2.022827831577287</v>
+        <v>2.022368597660459</v>
       </c>
       <c r="P3">
-        <v>171.79291</v>
+        <v>171.71772</v>
       </c>
       <c r="Q3">
-        <v>198.283323269072</v>
+        <v>198.287416170475</v>
       </c>
       <c r="R3">
-        <v>150.1753388285045</v>
+        <v>150.1504258470239</v>
       </c>
       <c r="S3">
-        <v>182.5866510926147</v>
+        <v>182.3819444923535</v>
       </c>
       <c r="T3">
-        <v>159.8489081499662</v>
+        <v>159.821941354878</v>
       </c>
       <c r="U3">
-        <v>0.04071665727812638</v>
+        <v>0.04073408270762569</v>
       </c>
       <c r="V3">
-        <v>0.04638597024649264</v>
+        <v>0.0463885921698482</v>
       </c>
       <c r="W3">
-        <v>0.03517530405324639</v>
+        <v>0.03518715254467193</v>
       </c>
       <c r="X3">
-        <v>0.04364018534902539</v>
+        <v>0.04365062156813727</v>
       </c>
       <c r="Y3">
-        <v>0.03767089855136178</v>
+        <v>0.03769072520242973</v>
       </c>
       <c r="Z3">
-        <v>0.6835048867934764</v>
+        <v>0.6835048984848644</v>
       </c>
       <c r="AA3">
-        <v>0.683506459686767</v>
+        <v>0.6835064434634854</v>
       </c>
       <c r="AB3">
-        <v>0.6835001748570466</v>
+        <v>0.6835002713780689</v>
       </c>
       <c r="AC3">
-        <v>0.6835052558197325</v>
+        <v>0.6835052668306218</v>
       </c>
       <c r="AD3">
-        <v>0.6835036889532036</v>
+        <v>0.6835037161834524</v>
       </c>
     </row>
     <row r="4" spans="1:30">
@@ -764,141 +764,141 @@
         <v>2.31</v>
       </c>
       <c r="P4">
-        <v>186.50467</v>
+        <v>186.11938</v>
       </c>
       <c r="Q4">
-        <v>331.2407210500325</v>
+        <v>331.1211714758743</v>
       </c>
       <c r="R4">
-        <v>124.636322010081</v>
+        <v>124.8773891949485</v>
       </c>
       <c r="S4">
-        <v>226.9763011706664</v>
+        <v>225.9438365158736</v>
       </c>
       <c r="T4">
-        <v>143.9597504461484</v>
+        <v>143.8209948344143</v>
       </c>
       <c r="U4">
-        <v>0.04206067033837396</v>
+        <v>0.04217750107223983</v>
       </c>
       <c r="V4">
-        <v>0.0986252985104932</v>
+        <v>0.09856727039136116</v>
       </c>
       <c r="W4">
-        <v>0.002945436653489209</v>
+        <v>0.002995157064678238</v>
       </c>
       <c r="X4">
-        <v>0.06889343880782478</v>
+        <v>0.06900750304990227</v>
       </c>
       <c r="Y4">
-        <v>0.01790480716131826</v>
+        <v>0.0179721845264825</v>
       </c>
       <c r="Z4">
-        <v>0.6474818659168552</v>
+        <v>0.6480967536251064</v>
       </c>
       <c r="AA4">
-        <v>0.8782783072232547</v>
+        <v>0.8788590562026701</v>
       </c>
       <c r="AB4">
-        <v>0.2953796257983124</v>
+        <v>0.2942739160203218</v>
       </c>
       <c r="AC4">
-        <v>0.775362019738978</v>
+        <v>0.7754857083400452</v>
       </c>
       <c r="AD4">
-        <v>0.4838502720253013</v>
+        <v>0.4845112728795999</v>
       </c>
     </row>
     <row r="5" spans="1:30">
       <c r="A5">
-        <v>0.3300331495893029</v>
+        <v>0.3297527023369954</v>
       </c>
       <c r="B5">
-        <v>0.3832382015488406</v>
+        <v>0.3835211989853209</v>
       </c>
       <c r="C5">
-        <v>0.2819127777249695</v>
+        <v>0.2820646983561017</v>
       </c>
       <c r="D5">
-        <v>0.3551205183965919</v>
+        <v>0.3548358448971214</v>
       </c>
       <c r="E5">
-        <v>0.3040084124808421</v>
+        <v>0.3036844575333699</v>
       </c>
       <c r="F5">
-        <v>6.997534177472011</v>
+        <v>6.99959957331527</v>
       </c>
       <c r="G5">
-        <v>8.846234874724741</v>
+        <v>8.822211548714666</v>
       </c>
       <c r="H5">
-        <v>5.457093860329499</v>
+        <v>5.468825961423108</v>
       </c>
       <c r="I5">
-        <v>7.830430822328724</v>
+        <v>7.833020355743384</v>
       </c>
       <c r="J5">
-        <v>6.125770669452572</v>
+        <v>6.128967116855383</v>
       </c>
       <c r="K5">
-        <v>2.309461781848148</v>
+        <v>2.308174082155408</v>
       </c>
       <c r="L5">
-        <v>3.042119375460159</v>
+        <v>3.036285692548471</v>
       </c>
       <c r="M5">
-        <v>1.714937588410952</v>
+        <v>1.71589277237482</v>
       </c>
       <c r="N5">
-        <v>2.635031083375674</v>
+        <v>2.633113997229116</v>
       </c>
       <c r="O5">
-        <v>1.970905978621198</v>
+        <v>1.967495510641607</v>
       </c>
       <c r="P5">
-        <v>186.88635</v>
+        <v>187.77498</v>
       </c>
       <c r="Q5">
-        <v>360.5627305333109</v>
+        <v>363.061766671988</v>
       </c>
       <c r="R5">
-        <v>108.4790183033491</v>
+        <v>108.7124494225298</v>
       </c>
       <c r="S5">
-        <v>236.597286836417</v>
+        <v>237.8216208933891</v>
       </c>
       <c r="T5">
-        <v>136.6659763557225</v>
+        <v>137.053414814629</v>
       </c>
       <c r="U5">
-        <v>0.04246358285443291</v>
+        <v>0.04215473926513635</v>
       </c>
       <c r="V5">
-        <v>0.103738989766315</v>
+        <v>0.103722803249861</v>
       </c>
       <c r="W5">
-        <v>0.001068415472739965</v>
+        <v>0.0009062563108073947</v>
       </c>
       <c r="X5">
-        <v>0.07153013296945986</v>
+        <v>0.07112792526370111</v>
       </c>
       <c r="Y5">
-        <v>0.01653668630498101</v>
+        <v>0.01641321719512654</v>
       </c>
       <c r="Z5">
-        <v>0.6399265389909821</v>
+        <v>0.6380592361797547</v>
       </c>
       <c r="AA5">
-        <v>0.894591287009132</v>
+        <v>0.8940501986107428</v>
       </c>
       <c r="AB5">
-        <v>0.2324892282248165</v>
+        <v>0.2299770683133065</v>
       </c>
       <c r="AC5">
-        <v>0.7812862996801779</v>
+        <v>0.7798247068670745</v>
       </c>
       <c r="AD5">
-        <v>0.4544817790281976</v>
+        <v>0.4523311835122468</v>
       </c>
     </row>
   </sheetData>

</xml_diff>